<commit_message>
TC22 Update for Prod Suite
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC22_Verify_PDP_Page.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC22_Verify_PDP_Page.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vaibhav Oza\KAMAN_ECTEST_IE_SANITY-master\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TC22_Verify_PDP_Page" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="54">
   <si>
     <t>TestCase</t>
   </si>
@@ -170,13 +175,13 @@
     <t>KamanDirectpartvalue</t>
   </si>
   <si>
-    <t>$83.82</t>
-  </si>
-  <si>
     <t>P2BSC100</t>
   </si>
   <si>
     <t>TC22_Verify_PDP_Page</t>
+  </si>
+  <si>
+    <t>$86.30</t>
   </si>
 </sst>
 </file>
@@ -264,7 +269,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -282,6 +287,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -293,6 +299,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -341,7 +350,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,7 +385,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -585,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +628,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>5</v>
@@ -640,69 +649,65 @@
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="B5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>8</v>
-      </c>
+      <c r="B6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>8</v>
@@ -710,12 +715,12 @@
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="2"/>
       <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>8</v>
@@ -724,11 +729,11 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>12</v>
+      <c r="C11" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>8</v>
@@ -737,170 +742,156 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="B12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="B13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
+      <c r="B14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="10" t="s">
-        <v>41</v>
+      <c r="B18" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>22</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="10" t="s">
-        <v>41</v>
+      <c r="B20" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="9" t="s">
-        <v>16</v>
+      <c r="B21" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="10" t="s">
-        <v>41</v>
+      <c r="B22" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="9" t="s">
-        <v>16</v>
+      <c r="B23" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,28 +900,28 @@
         <v>16</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="9" t="s">
-        <v>16</v>
+      <c r="B25" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -939,13 +930,13 @@
         <v>16</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -954,28 +945,28 @@
         <v>16</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="9" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -984,92 +975,92 @@
         <v>16</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="9" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="6"/>
+      <c r="B31" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="9" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B34" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>30</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
@@ -1077,23 +1068,29 @@
         <v>16</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
@@ -1101,13 +1098,13 @@
         <v>16</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1116,13 +1113,13 @@
         <v>16</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1131,7 +1128,7 @@
         <v>20</v>
       </c>
       <c r="C40" s="6"/>
-      <c r="D40" s="8"/>
+      <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1140,13 +1137,13 @@
         <v>16</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1155,12 +1152,51 @@
         <v>16</v>
       </c>
       <c r="C42" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="6" t="s">
+      <c r="D45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1173,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,7 +1272,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1332,7 +1368,7 @@
         <v>50</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>